<commit_message>
Updated modules acc to LicenseKey
</commit_message>
<xml_diff>
--- a/Reports/2025_05_CanteenReports.xlsx
+++ b/Reports/2025_05_CanteenReports.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="7" customWidth="1" min="3" max="3"/>
     <col width="7" customWidth="1" min="4" max="4"/>
-    <col width="7" customWidth="1" min="5" max="5"/>
-    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="5" customWidth="1" min="6" max="6"/>
     <col width="7" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -470,27 +470,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>BREAKFAST</t>
+          <t>DINNER</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>KHAANA</t>
+          <t>LUNCH</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>LUNCH</t>
+          <t>PIZZA</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>SNACK</t>
+          <t>SNACKS</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>SNACKS</t>
+          <t>TEA</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -502,151 +502,76 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>22-05-2025</t>
+          <t>29-05-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>23-05-2025</t>
+          <t>31-05-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>154</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>157</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>26-05-2025</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>27-05-2025</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="G5" s="3" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>28-05-2025</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>88</v>
-      </c>
-      <c r="E6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3" t="n">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="inlineStr">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B7" s="5" t="n">
-        <v>210</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>91</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F7" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="G7" s="5" t="n">
-        <v>315</v>
+      <c r="B4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -660,7 +585,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -672,11 +597,11 @@
     <col width="7" customWidth="1" min="2" max="2"/>
     <col width="9" customWidth="1" min="3" max="3"/>
     <col width="6" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="7" customWidth="1" min="6" max="6"/>
     <col width="7" customWidth="1" min="7" max="7"/>
-    <col width="7" customWidth="1" min="8" max="8"/>
-    <col width="8" customWidth="1" min="9" max="9"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
+    <col width="5" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -702,27 +627,27 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>BREAKFAST</t>
+          <t>DINNER</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>KHAANA</t>
+          <t>LUNCH</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>LUNCH</t>
+          <t>PIZZA</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>SNACK</t>
+          <t>SNACKS</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>SNACKS</t>
+          <t>TEA</t>
         </is>
       </c>
     </row>
@@ -734,48 +659,75 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="inlineStr"/>
       <c r="E2" s="3" t="n">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="H2" s="3" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I2" s="3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr"/>
-      <c r="B3" s="4" t="inlineStr"/>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="A3" s="2" t="n">
+        <v>2025</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="inlineStr"/>
+      <c r="E3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr"/>
+      <c r="B4" s="4" t="inlineStr"/>
+      <c r="C4" s="4" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="D3" s="4" t="inlineStr"/>
-      <c r="E3" s="5" t="n">
-        <v>210</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="G3" s="5" t="n">
-        <v>91</v>
-      </c>
-      <c r="H3" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="I3" s="5" t="n">
-        <v>3</v>
+      <c r="D4" s="4" t="inlineStr"/>
+      <c r="E4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -789,7 +741,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH6"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -798,7 +750,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="10" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="3" customWidth="1" min="4" max="4"/>
     <col width="3" customWidth="1" min="5" max="5"/>
@@ -822,7 +774,7 @@
     <col width="4" customWidth="1" min="23" max="23"/>
     <col width="4" customWidth="1" min="24" max="24"/>
     <col width="4" customWidth="1" min="25" max="25"/>
-    <col width="5" customWidth="1" min="26" max="26"/>
+    <col width="4" customWidth="1" min="26" max="26"/>
     <col width="4" customWidth="1" min="27" max="27"/>
     <col width="4" customWidth="1" min="28" max="28"/>
     <col width="4" customWidth="1" min="29" max="29"/>
@@ -1008,16 +960,16 @@
     <row r="2">
       <c r="A2" s="4" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>BREAKFAST</t>
+          <t>LUNCH</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="inlineStr"/>
       <c r="E2" s="2" t="inlineStr"/>
@@ -1040,34 +992,32 @@
       <c r="V2" s="2" t="inlineStr"/>
       <c r="W2" s="2" t="inlineStr"/>
       <c r="X2" s="2" t="inlineStr"/>
-      <c r="Y2" s="2" t="n">
-        <v>49</v>
-      </c>
-      <c r="Z2" s="2" t="n">
-        <v>154</v>
-      </c>
+      <c r="Y2" s="2" t="inlineStr"/>
+      <c r="Z2" s="2" t="inlineStr"/>
       <c r="AA2" s="2" t="inlineStr"/>
       <c r="AB2" s="2" t="inlineStr"/>
-      <c r="AC2" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="AD2" s="2" t="n">
-        <v>4</v>
-      </c>
+      <c r="AC2" s="2" t="inlineStr"/>
+      <c r="AD2" s="2" t="inlineStr"/>
       <c r="AE2" s="2" t="inlineStr"/>
       <c r="AF2" s="2" t="inlineStr"/>
       <c r="AG2" s="2" t="inlineStr"/>
-      <c r="AH2" s="2" t="inlineStr"/>
+      <c r="AH2" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr"/>
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>KHAANA</t>
+          <t>DINNER</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="inlineStr"/>
       <c r="E3" s="2" t="inlineStr"/>
@@ -1090,9 +1040,7 @@
       <c r="V3" s="2" t="inlineStr"/>
       <c r="W3" s="2" t="inlineStr"/>
       <c r="X3" s="2" t="inlineStr"/>
-      <c r="Y3" s="2" t="n">
-        <v>4</v>
-      </c>
+      <c r="Y3" s="2" t="inlineStr"/>
       <c r="Z3" s="2" t="inlineStr"/>
       <c r="AA3" s="2" t="inlineStr"/>
       <c r="AB3" s="2" t="inlineStr"/>
@@ -1101,7 +1049,9 @@
       <c r="AE3" s="2" t="inlineStr"/>
       <c r="AF3" s="2" t="inlineStr"/>
       <c r="AG3" s="2" t="inlineStr"/>
-      <c r="AH3" s="2" t="inlineStr"/>
+      <c r="AH3" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr"/>
@@ -1111,7 +1061,7 @@
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>91</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="inlineStr"/>
       <c r="E4" s="2" t="inlineStr"/>
@@ -1135,29 +1085,27 @@
       <c r="W4" s="2" t="inlineStr"/>
       <c r="X4" s="2" t="inlineStr"/>
       <c r="Y4" s="2" t="inlineStr"/>
-      <c r="Z4" s="2" t="n">
-        <v>3</v>
-      </c>
+      <c r="Z4" s="2" t="inlineStr"/>
       <c r="AA4" s="2" t="inlineStr"/>
       <c r="AB4" s="2" t="inlineStr"/>
       <c r="AC4" s="2" t="inlineStr"/>
       <c r="AD4" s="2" t="inlineStr"/>
-      <c r="AE4" s="2" t="n">
-        <v>88</v>
-      </c>
+      <c r="AE4" s="2" t="inlineStr"/>
       <c r="AF4" s="2" t="inlineStr"/>
       <c r="AG4" s="2" t="inlineStr"/>
-      <c r="AH4" s="2" t="inlineStr"/>
+      <c r="AH4" s="2" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr"/>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>SNACK</t>
+          <t>PIZZA</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="inlineStr"/>
       <c r="E5" s="2" t="inlineStr"/>
@@ -1180,9 +1128,7 @@
       <c r="V5" s="2" t="inlineStr"/>
       <c r="W5" s="2" t="inlineStr"/>
       <c r="X5" s="2" t="inlineStr"/>
-      <c r="Y5" s="2" t="n">
-        <v>7</v>
-      </c>
+      <c r="Y5" s="2" t="inlineStr"/>
       <c r="Z5" s="2" t="inlineStr"/>
       <c r="AA5" s="2" t="inlineStr"/>
       <c r="AB5" s="2" t="inlineStr"/>
@@ -1191,7 +1137,9 @@
       <c r="AE5" s="2" t="inlineStr"/>
       <c r="AF5" s="2" t="inlineStr"/>
       <c r="AG5" s="2" t="inlineStr"/>
-      <c r="AH5" s="2" t="inlineStr"/>
+      <c r="AH5" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr"/>
@@ -1201,7 +1149,7 @@
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2" t="inlineStr"/>
       <c r="E6" s="2" t="inlineStr"/>
@@ -1229,13 +1177,61 @@
       <c r="AA6" s="2" t="inlineStr"/>
       <c r="AB6" s="2" t="inlineStr"/>
       <c r="AC6" s="2" t="inlineStr"/>
-      <c r="AD6" s="2" t="n">
-        <v>3</v>
-      </c>
+      <c r="AD6" s="2" t="inlineStr"/>
       <c r="AE6" s="2" t="inlineStr"/>
-      <c r="AF6" s="2" t="inlineStr"/>
+      <c r="AF6" s="2" t="n">
+        <v>6</v>
+      </c>
       <c r="AG6" s="2" t="inlineStr"/>
-      <c r="AH6" s="2" t="inlineStr"/>
+      <c r="AH6" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr"/>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>TEA</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="inlineStr"/>
+      <c r="E7" s="2" t="inlineStr"/>
+      <c r="F7" s="2" t="inlineStr"/>
+      <c r="G7" s="2" t="inlineStr"/>
+      <c r="H7" s="2" t="inlineStr"/>
+      <c r="I7" s="2" t="inlineStr"/>
+      <c r="J7" s="2" t="inlineStr"/>
+      <c r="K7" s="2" t="inlineStr"/>
+      <c r="L7" s="2" t="inlineStr"/>
+      <c r="M7" s="2" t="inlineStr"/>
+      <c r="N7" s="2" t="inlineStr"/>
+      <c r="O7" s="2" t="inlineStr"/>
+      <c r="P7" s="2" t="inlineStr"/>
+      <c r="Q7" s="2" t="inlineStr"/>
+      <c r="R7" s="2" t="inlineStr"/>
+      <c r="S7" s="2" t="inlineStr"/>
+      <c r="T7" s="2" t="inlineStr"/>
+      <c r="U7" s="2" t="inlineStr"/>
+      <c r="V7" s="2" t="inlineStr"/>
+      <c r="W7" s="2" t="inlineStr"/>
+      <c r="X7" s="2" t="inlineStr"/>
+      <c r="Y7" s="2" t="inlineStr"/>
+      <c r="Z7" s="2" t="inlineStr"/>
+      <c r="AA7" s="2" t="inlineStr"/>
+      <c r="AB7" s="2" t="inlineStr"/>
+      <c r="AC7" s="2" t="inlineStr"/>
+      <c r="AD7" s="2" t="inlineStr"/>
+      <c r="AE7" s="2" t="inlineStr"/>
+      <c r="AF7" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG7" s="2" t="inlineStr"/>
+      <c r="AH7" s="2" t="n">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>